<commit_message>
DB creation and update
</commit_message>
<xml_diff>
--- a/messi_goals.xlsx
+++ b/messi_goals.xlsx
@@ -440,7 +440,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>#_of_Goal</t>
+          <t>N_of_Goal</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -450,12 +450,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Home team</t>
+          <t>Home_team</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Away team</t>
+          <t>Away_team</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Home/Away</t>
+          <t>Home_or_Away</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">

</xml_diff>